<commit_message>
Script junio y 1er sac
</commit_message>
<xml_diff>
--- a/Pagos Eventuales realizados/06- JUNIO/Agentes a pagar 8.6.23.xlsx
+++ b/Pagos Eventuales realizados/06- JUNIO/Agentes a pagar 8.6.23.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>Nro control</t>
   </si>
@@ -97,6 +97,51 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Gratificacion 3ra cuota 2021 (diciembre 21)</t>
+  </si>
+  <si>
+    <t>Gratificacion 2021 3ra cuota Diciembre</t>
+  </si>
+  <si>
+    <t>12/21</t>
+  </si>
+  <si>
+    <t>EX-2021-2819564--GDESDE-MS</t>
+  </si>
+  <si>
+    <t>NO-2023-05108774-GDESDE-HRE#MS</t>
+  </si>
+  <si>
+    <t>27303538025</t>
+  </si>
+  <si>
+    <t>38989814</t>
+  </si>
+  <si>
+    <t>RODRIGUEZ NELIDA BEATRIZ</t>
+  </si>
+  <si>
+    <t>38566661</t>
+  </si>
+  <si>
+    <t>PERALTA CARLOS RODOLFO</t>
+  </si>
+  <si>
+    <t>CACERES GUSTAVO ADOLFO</t>
+  </si>
+  <si>
+    <t>LUDUENIA MILENA</t>
+  </si>
+  <si>
+    <t>20386401560</t>
+  </si>
+  <si>
+    <t>29054282</t>
+  </si>
+  <si>
+    <t>JOZAME GIMENEZ JORGE A</t>
   </si>
 </sst>
 </file>
@@ -136,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,8 +206,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -209,18 +260,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -260,12 +323,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,11 +641,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,454 +692,474 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="27"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="15">
+        <v>20205475800</v>
+      </c>
+      <c r="D3" s="15">
+        <v>77214112</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="15">
+        <v>30000</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="21">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="22">
+        <f>SUM(F3)</f>
+        <v>30000</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="7" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F6" s="33">
         <v>25000</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G6" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="18" t="s">
+      <c r="H6" s="34"/>
+      <c r="I6" s="35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="22">
+    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
+      <c r="B7" s="36">
         <v>1</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="23">
-        <f>SUM(F3)</f>
-        <v>25000</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="16">
-        <v>25000</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="22">
-        <v>1</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="23">
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="39">
         <f>SUM(F6)</f>
         <v>25000</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="9"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="40"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="31"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="33">
+        <v>25000</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="34"/>
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="36">
+        <v>1</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="39">
+        <f>SUM(F9)</f>
+        <v>25000</v>
+      </c>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="40"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="7" t="s">
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="13" t="s">
+      <c r="C12" s="15">
+        <v>27387805961</v>
+      </c>
+      <c r="D12" s="18">
+        <v>77326215</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F12" s="11">
         <v>60000</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="18" t="s">
+      <c r="H12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="20"/>
-    </row>
-    <row r="10" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="22">
-        <v>19</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="23">
-        <f>SUM(F9:F10)</f>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="11">
         <v>60000</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="G13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="28">
+        <v>20140300676</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="11">
+        <v>60000</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="21">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="22">
+        <f>SUM(F12:F14)</f>
+        <v>180000</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
-      <c r="B14" s="7" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="8" t="s">
+      <c r="C18" s="15">
+        <v>27387805961</v>
+      </c>
+      <c r="D18" s="15">
+        <v>77326215</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F18" s="6">
         <v>80000</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="18" t="s">
+      <c r="H18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="7" t="s">
+      <c r="J18" s="29"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="8" t="s">
+      <c r="C19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F19" s="6">
         <v>80000</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="18" t="s">
+      <c r="H19" s="26"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="6">
+        <v>80000</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="26"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="21">
+        <v>3</v>
+      </c>
+      <c r="F21" s="22">
+        <f>SUM(F18:F20)</f>
+        <v>240000</v>
+      </c>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="15">
+        <v>27387805961</v>
+      </c>
+      <c r="D24" s="15">
+        <v>77326215</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="6">
+        <v>60000</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="22">
-        <v>19</v>
-      </c>
-      <c r="F16" s="23">
-        <f>SUM(F14:F15)</f>
-        <v>160000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="7" t="s">
+      <c r="J24" s="23"/>
+    </row>
+    <row r="25" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="8" t="s">
+      <c r="C25" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F25" s="6">
         <v>60000</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="24"/>
-    </row>
-    <row r="20" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="24"/>
-    </row>
-    <row r="21" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="24"/>
-    </row>
-    <row r="22" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="24"/>
-    </row>
-    <row r="23" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="24"/>
-    </row>
-    <row r="24" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="24"/>
-    </row>
-    <row r="25" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="24"/>
-    </row>
-    <row r="26" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="24"/>
-    </row>
-    <row r="27" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="24"/>
-    </row>
-    <row r="28" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="24"/>
-    </row>
-    <row r="29" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="24"/>
-    </row>
-    <row r="30" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="24"/>
-    </row>
-    <row r="31" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="24"/>
-    </row>
-    <row r="32" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="26"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="24"/>
-    </row>
-    <row r="33" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="24"/>
-    </row>
-    <row r="34" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="24"/>
-    </row>
-    <row r="35" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="24"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="14"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B37" s="22">
-        <v>18</v>
-      </c>
-      <c r="F37" s="23">
-        <f>SUM(F18:F36)</f>
+      <c r="H25" s="26"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="23"/>
+    </row>
+    <row r="26" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="6">
         <v>60000</v>
       </c>
+      <c r="G26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="26"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="23"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="21">
+        <v>3</v>
+      </c>
+      <c r="F27" s="22">
+        <f>SUM(F24:F26)</f>
+        <v>180000</v>
+      </c>
+      <c r="H27" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>